<commit_message>
Add the diffusion and tracked calculations
</commit_message>
<xml_diff>
--- a/cluster/data test/dist-change-homer-ampar-LTD-1.xlsx
+++ b/cluster/data test/dist-change-homer-ampar-LTD-1.xlsx
@@ -370,836 +370,1145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369A72CF-A55F-4E18-AE19-C59819C29B49}">
-  <dimension ref="A1:B103"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B103"/>
+      <selection sqref="A1:C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2624.0806173769979</v>
       </c>
       <c r="B1">
         <v>9524.7957881147031</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>39.661576838990712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>588.32574505585046</v>
       </c>
       <c r="B2">
         <v>8434.8251497599558</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>295.76621513053516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3317.1437276983675</v>
       </c>
       <c r="B3">
         <v>3725.340686887359</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>74.733977165428001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5085.3004634418285</v>
       </c>
       <c r="B4">
         <v>5148.3970046068844</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>126.88069883751206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13250.750267824465</v>
       </c>
       <c r="B5">
         <v>11610.19395226664</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>130.20867875123534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5287.360921062299</v>
       </c>
       <c r="B6">
         <v>314.91327135224623</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>430.88892641510722</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9824.2974636714425</v>
       </c>
       <c r="B7">
         <v>6560.5858266538835</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>254.26403544915837</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1121.5732642156418</v>
       </c>
       <c r="B8">
         <v>3506.5316397287911</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>94.801936647429827</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4494.4030435008654</v>
       </c>
       <c r="B9">
         <v>6699.4002354842369</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>143.23278033753741</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>310.36181206206425</v>
       </c>
       <c r="B10">
         <v>313.89028197030899</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>117.75149697655652</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>244.64174484642768</v>
       </c>
       <c r="B11">
         <v>6872.6497171360743</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>258.60655480161415</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5163.6188792312651</v>
       </c>
       <c r="B12">
         <v>5252.4852626135371</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>52.443698438959167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>130.42171510243892</v>
       </c>
       <c r="B13">
         <v>137.1344122572898</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>27.074246049955519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>307.70029280697514</v>
       </c>
       <c r="B14">
         <v>9372.0011731486684</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>257.87275622842628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1008.5940719816466</v>
       </c>
       <c r="B15">
         <v>214.4827666257633</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>33.04314485073985</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1784.5571691272585</v>
       </c>
       <c r="B16">
         <v>7688.14024632368</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>173.33989559288116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4965.1248449634986</v>
       </c>
       <c r="B17">
         <v>4071.754689630166</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>208.17209941609539</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>579.94281625091924</v>
       </c>
       <c r="B18">
         <v>9903.74538761445</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>757.10632321431433</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>112.29757675098161</v>
       </c>
       <c r="B19">
         <v>185.88474707270225</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>163.14034917521431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4715.2436369300385</v>
       </c>
       <c r="B20">
         <v>6717.7468295892149</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>89.559845473220037</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1889.1357348019321</v>
       </c>
       <c r="B21">
         <v>6188.6120454540787</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>128.72229685243937</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1886.4858539156044</v>
       </c>
       <c r="B22">
         <v>303.44124428175741</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>128.43969387593808</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1284.6082827195837</v>
       </c>
       <c r="B23">
         <v>1619.8174617941606</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>225.89213287039405</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6187.8016896931267</v>
       </c>
       <c r="B24">
         <v>4431.834771726406</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>82.947213971479798</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>433.64715971694596</v>
       </c>
       <c r="B25">
         <v>3608.0183359692855</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>113.44491440584073</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2319.4226365624945</v>
       </c>
       <c r="B26">
         <v>6327.7295838780592</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>5358.6679975083171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>11525.735196961828</v>
       </c>
       <c r="B27">
         <v>8627.5241078341805</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>58.803254715400463</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3334.8345564743854</v>
       </c>
       <c r="B28">
         <v>3062.6683120052735</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>260.54709154766317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2441.1174314536529</v>
       </c>
       <c r="B29">
         <v>6312.7182029407477</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>203.6717821177281</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>596.66625056666601</v>
       </c>
       <c r="B30">
         <v>2745.0642537282361</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>265.07027376910264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5619.8043489291431</v>
       </c>
       <c r="B31">
         <v>5782.7517167848746</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>345.49898453816445</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3055.3679985294784</v>
       </c>
       <c r="B32">
         <v>1733.6124260877193</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>104.6751717930136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3508.5065730528695</v>
       </c>
       <c r="B33">
         <v>4458.8373652354076</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>68.329405730533367</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4008.8549200398666</v>
       </c>
       <c r="B34">
         <v>3667.1893605185051</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>160.5091910730176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3903.6177886722071</v>
       </c>
       <c r="B35">
         <v>6008.8935043522506</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>163.86053316942341</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1135.6755525579056</v>
       </c>
       <c r="B36">
         <v>3148.6464265795548</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>531.99168167310359</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3311.0415585536066</v>
       </c>
       <c r="B37">
         <v>4685.7304718676478</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>46.942016262882142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>361.49290621698879</v>
       </c>
       <c r="B38">
         <v>174.32435710229811</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>159.23440579921328</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2238.414445195353</v>
       </c>
       <c r="B39">
         <v>3037.3621166166408</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>113.72894733620301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8293.1674748542173</v>
       </c>
       <c r="B40">
         <v>5655.9497290635645</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>744.04509883765877</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>414.94095572016215</v>
       </c>
       <c r="B41">
         <v>714.1833802495072</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>224.41242259378564</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6533.2327833391018</v>
       </c>
       <c r="B42">
         <v>6223.4623050062637</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>268.72760405871361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>168.8156363070074</v>
       </c>
       <c r="B43">
         <v>8469.2385679625622</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>135.25711848068877</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2534.3862871043584</v>
       </c>
       <c r="B44">
         <v>8384.4091697207896</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>187.89376781094867</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3192.1492986816497</v>
       </c>
       <c r="B45">
         <v>3153.7253989574915</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>233.5135551461384</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2571.2914416053227</v>
       </c>
       <c r="B46">
         <v>198.46762930452209</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>51.13615847776105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2925.6415650263175</v>
       </c>
       <c r="B47">
         <v>1516.9988467483556</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>242.75865789689698</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>352.76110857958736</v>
       </c>
       <c r="B48">
         <v>743.47447429787667</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>361.93790454455956</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>8063.3490043360807</v>
       </c>
       <c r="B49">
         <v>9983.0622968700191</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>204.24147580917403</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>182.0466216591488</v>
       </c>
       <c r="B50">
         <v>7723.0602588185311</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>136.86445181394473</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3402.2859285718887</v>
       </c>
       <c r="B51">
         <v>2942.170502472065</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>398.70533643903451</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5902.4056303854941</v>
       </c>
       <c r="B52">
         <v>6765.1219110847778</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>35.837263721126227</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>567.00234914135422</v>
       </c>
       <c r="B53">
         <v>2156.1457123250211</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>476.16138808071042</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3137.6235680057844</v>
       </c>
       <c r="B54">
         <v>8707.3532606278641</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>389.02315538207284</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5563.0525113248095</v>
       </c>
       <c r="B55">
         <v>5140.1048816308057</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>352.51787408860872</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5176.4747125074282</v>
       </c>
       <c r="B56">
         <v>10440.311326163508</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>572.3550149539177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9825.4426913760672</v>
       </c>
       <c r="B57">
         <v>1970.3356726222644</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>83.052129353280222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1341.4240849587641</v>
       </c>
       <c r="B58">
         <v>1413.831894897186</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>151.18084098533325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6270.0565495501878</v>
       </c>
       <c r="B59">
         <v>8909.681663720954</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>323.08532054171104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4628.6082404924791</v>
       </c>
       <c r="B60">
         <v>5318.1054209937811</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>185.2535526837807</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>153.18298400143058</v>
       </c>
       <c r="B61">
         <v>230.4108130298689</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>106.09015401974783</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1487.1614846408127</v>
       </c>
       <c r="B62">
         <v>9702.6979137178332</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>185.00269291138164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2780.7378458390672</v>
       </c>
       <c r="B63">
         <v>2596.6645792618897</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>85.741034010410914</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3697.0480890924896</v>
       </c>
       <c r="B64">
         <v>1787.0034976133784</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>652.21707044179755</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>10647.30590586709</v>
       </c>
       <c r="B65">
         <v>10789.740678163556</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>373.67707282607932</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>13092.81778906275</v>
       </c>
       <c r="B66">
         <v>19440.783574993045</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>14809.972877809972</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>216.82386136401161</v>
       </c>
       <c r="B67">
         <v>4462.7286024636414</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>133.82224093694566</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3336.2892347975089</v>
       </c>
       <c r="B68">
         <v>5808.7755097631871</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>251.80782104352272</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2319.4226365624945</v>
       </c>
       <c r="B69">
         <v>8798.6145702100657</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>133.06565696596417</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>8293.1674748542173</v>
       </c>
       <c r="B70">
         <v>4851.016974469102</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>457.52493923349601</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5001.8650160786128</v>
       </c>
       <c r="B71">
         <v>4269.6884357323215</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>134.84257473493412</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>940.93450333421504</v>
       </c>
       <c r="B72">
         <v>4273.7452517029415</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>115.27995318571632</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>182.0466216591488</v>
       </c>
       <c r="B73">
         <v>8861.5347799911269</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>3571.4904413068298</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1402.2040759169672</v>
       </c>
       <c r="B74">
         <v>7076.5048348912487</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>1467.4656695062847</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5176.4747125074282</v>
       </c>
       <c r="B75">
         <v>11951.921012963083</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>1136.849486141376</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>197.25975950617641</v>
       </c>
       <c r="B76">
         <v>2217.0051974879166</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>526.75866053598588</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3041.1995376832829</v>
       </c>
       <c r="B77">
         <v>4593.8583850152036</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>75.165634690516313</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4571.535988925074</v>
       </c>
       <c r="B78">
         <v>4376.2187273356603</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>63.283667760863146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>6533.2327833391018</v>
       </c>
       <c r="B79">
         <v>5296.9812817330212</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>2729.143040590036</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>307.70029280697514</v>
       </c>
       <c r="B80">
         <v>17371.273835137341</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>14824.323764916691</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2958.6084225483442</v>
       </c>
       <c r="B81">
         <v>1759.7494865464378</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>695.62553332888876</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1023.5136871242453</v>
       </c>
       <c r="B82">
         <v>7157.1830831288917</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>99.528070339120518</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1072.921699765358</v>
       </c>
       <c r="B83">
         <v>2329.1611215967027</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>107.16072071101756</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2165.7869172730598</v>
       </c>
       <c r="B84">
         <v>106.38081574191705</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>66.204617619713545</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>3153.9817811783746</v>
       </c>
       <c r="B85">
         <v>4145.9863073018241</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>169.54592441811812</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1305.538114233839</v>
       </c>
       <c r="B86">
         <v>1391.3584300876983</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>1855.3326954348984</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>187.74146964875362</v>
       </c>
       <c r="B87">
         <v>5700.2078259474138</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>86.891437461189696</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1305.538114233839</v>
       </c>
       <c r="B88">
         <v>650.90917168367707</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>66.915592483345065</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2508.5294517692023</v>
       </c>
       <c r="B89">
         <v>2387.4421228550582</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>76.748618130886641</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1625.7977156434401</v>
       </c>
       <c r="B90">
         <v>3145.8794664690818</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>2889.9817903173771</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1023.5136871242453</v>
       </c>
       <c r="B91">
         <v>11278.047359650049</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>6148.1391984159764</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>153.18298400143058</v>
       </c>
       <c r="B92">
         <v>2484.4330444381903</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>2294.2269463621556</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>4005.5471191969204</v>
       </c>
       <c r="B93">
         <v>5589.7974998000409</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>51.869931312899503</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>4972.9986707021035</v>
       </c>
       <c r="B94">
         <v>9380.0695423927773</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>180.69882251811921</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2127.6421034976565</v>
       </c>
       <c r="B95">
         <v>6760.3179456368034</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>120.24099369651071</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1023.5136871242453</v>
       </c>
       <c r="B96">
         <v>7524.0360788626986</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>1665.2022897403235</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1997.72348636639</v>
       </c>
       <c r="B97">
         <v>3916.9975801305359</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>92.96112726645039</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>4370.0961656887139</v>
       </c>
       <c r="B98">
         <v>3523.3423574757439</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>1434.4389208812911</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1305.538114233839</v>
       </c>
       <c r="B99">
         <v>1811.7848566601581</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>2001.7734309749542</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1327.3460432984918</v>
       </c>
       <c r="B100">
         <v>211.83067468196899</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>47.640038874502579</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>827.15078313528306</v>
       </c>
       <c r="B101">
         <v>3692.0682678579724</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>1138.5603361865105</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1574.6274536852238</v>
       </c>
       <c r="B102">
         <v>1627.2054424463449</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <v>127.60089229038861</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>248.32944211166716</v>
       </c>
       <c r="B103">
         <v>1699.981552183418</v>
+      </c>
+      <c r="C103">
+        <v>1690.208403760899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>